<commit_message>
Update timewarp to support daily files and aggregate monthly reports
- Generate daily Excel files with timestamp (orari_lavoro_YYYYMMDD.xlsx)
- Aggregate data from all daily files for monthly reports
- Create separate summary file (orari_riepilogo_mensile.xlsx) for monthly charts
- Improve file handling and state management

🤖 Generated with [Claude Code](https://claude.com/claude-code)

Co-Authored-By: Claude <noreply@anthropic.com>
</commit_message>
<xml_diff>
--- a/orari_lavoro.xlsx
+++ b/orari_lavoro.xlsx
@@ -339,6 +339,220 @@
 </chartSpace>
 </file>
 
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns="http://schemas.openxmlformats.org/drawingml/2006/chart">
+  <chart>
+    <title>
+      <tx>
+        <rich>
+          <a:bodyPr/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:t>Ore lavorate per mese</a:t>
+            </a:r>
+          </a:p>
+        </rich>
+      </tx>
+    </title>
+    <plotArea>
+      <barChart>
+        <barDir val="col"/>
+        <grouping val="clustered"/>
+        <ser>
+          <idx val="0"/>
+          <order val="0"/>
+          <spPr>
+            <a:ln>
+              <a:prstDash val="solid"/>
+            </a:ln>
+          </spPr>
+          <cat>
+            <numRef>
+              <f>'Mensile'!$A$2</f>
+            </numRef>
+          </cat>
+          <val>
+            <numRef>
+              <f>'Mensile'!$B$2</f>
+            </numRef>
+          </val>
+        </ser>
+        <gapWidth val="150"/>
+        <axId val="10"/>
+        <axId val="100"/>
+      </barChart>
+      <catAx>
+        <axId val="10"/>
+        <scaling>
+          <orientation val="minMax"/>
+        </scaling>
+        <axPos val="l"/>
+        <title>
+          <tx>
+            <rich>
+              <a:bodyPr/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:t>Mese</a:t>
+                </a:r>
+              </a:p>
+            </rich>
+          </tx>
+        </title>
+        <majorTickMark val="none"/>
+        <minorTickMark val="none"/>
+        <crossAx val="100"/>
+        <lblOffset val="100"/>
+      </catAx>
+      <valAx>
+        <axId val="100"/>
+        <scaling>
+          <orientation val="minMax"/>
+        </scaling>
+        <axPos val="l"/>
+        <majorGridlines/>
+        <title>
+          <tx>
+            <rich>
+              <a:bodyPr/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:t>Ore Totali</a:t>
+                </a:r>
+              </a:p>
+            </rich>
+          </tx>
+        </title>
+        <majorTickMark val="none"/>
+        <minorTickMark val="none"/>
+        <crossAx val="10"/>
+      </valAx>
+    </plotArea>
+    <legend>
+      <legendPos val="r"/>
+    </legend>
+    <plotVisOnly val="1"/>
+    <dispBlanksAs val="gap"/>
+  </chart>
+</chartSpace>
+</file>
+
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns="http://schemas.openxmlformats.org/drawingml/2006/chart">
+  <chart>
+    <title>
+      <tx>
+        <rich>
+          <a:bodyPr/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:t>Ore lavorate per mese</a:t>
+            </a:r>
+          </a:p>
+        </rich>
+      </tx>
+    </title>
+    <plotArea>
+      <barChart>
+        <barDir val="col"/>
+        <grouping val="clustered"/>
+        <ser>
+          <idx val="0"/>
+          <order val="0"/>
+          <spPr>
+            <a:ln>
+              <a:prstDash val="solid"/>
+            </a:ln>
+          </spPr>
+          <cat>
+            <numRef>
+              <f>'Mensile'!$A$2</f>
+            </numRef>
+          </cat>
+          <val>
+            <numRef>
+              <f>'Mensile'!$B$2</f>
+            </numRef>
+          </val>
+        </ser>
+        <gapWidth val="150"/>
+        <axId val="10"/>
+        <axId val="100"/>
+      </barChart>
+      <catAx>
+        <axId val="10"/>
+        <scaling>
+          <orientation val="minMax"/>
+        </scaling>
+        <axPos val="l"/>
+        <title>
+          <tx>
+            <rich>
+              <a:bodyPr/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:t>Mese</a:t>
+                </a:r>
+              </a:p>
+            </rich>
+          </tx>
+        </title>
+        <majorTickMark val="none"/>
+        <minorTickMark val="none"/>
+        <crossAx val="100"/>
+        <lblOffset val="100"/>
+      </catAx>
+      <valAx>
+        <axId val="100"/>
+        <scaling>
+          <orientation val="minMax"/>
+        </scaling>
+        <axPos val="l"/>
+        <majorGridlines/>
+        <title>
+          <tx>
+            <rich>
+              <a:bodyPr/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:t>Ore Totali</a:t>
+                </a:r>
+              </a:p>
+            </rich>
+          </tx>
+        </title>
+        <majorTickMark val="none"/>
+        <minorTickMark val="none"/>
+        <crossAx val="10"/>
+      </valAx>
+    </plotArea>
+    <legend>
+      <legendPos val="r"/>
+    </legend>
+    <plotVisOnly val="1"/>
+    <dispBlanksAs val="gap"/>
+  </chart>
+</chartSpace>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <wsDr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
   <oneCellAnchor>
@@ -385,6 +599,50 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </graphicFrame>
+    <clientData/>
+  </oneCellAnchor>
+  <oneCellAnchor>
+    <from>
+      <col>3</col>
+      <colOff>0</colOff>
+      <row>1</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="5400000" cy="2700000"/>
+    <graphicFrame>
+      <nvGraphicFramePr>
+        <cNvPr id="2" name="Chart 2"/>
+        <cNvGraphicFramePr/>
+      </nvGraphicFramePr>
+      <xfrm/>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </graphicFrame>
+    <clientData/>
+  </oneCellAnchor>
+  <oneCellAnchor>
+    <from>
+      <col>3</col>
+      <colOff>0</colOff>
+      <row>1</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="5400000" cy="2700000"/>
+    <graphicFrame>
+      <nvGraphicFramePr>
+        <cNvPr id="3" name="Chart 3"/>
+        <cNvGraphicFramePr/>
+      </nvGraphicFramePr>
+      <xfrm/>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart r:id="rId3"/>
         </a:graphicData>
       </a:graphic>
     </graphicFrame>
@@ -682,7 +940,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E4"/>
+  <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -790,6 +1048,56 @@
       </c>
       <c r="E4" t="n">
         <v>8</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>2025-11-20</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>Magazzino</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>12:00</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>16:00</t>
+        </is>
+      </c>
+      <c r="E5" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>2025-11-18</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>Produzione</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>12:00</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>16:00</t>
+        </is>
+      </c>
+      <c r="E6" t="n">
+        <v>4</v>
       </c>
     </row>
   </sheetData>
@@ -831,7 +1139,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>16</v>
+        <v>24</v>
       </c>
     </row>
   </sheetData>

</xml_diff>